<commit_message>
correcting problems with name changes
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_fullrun_hbrown_11.11.19.xlsx
+++ b/fastqFiles/fastq_fullrun_hbrown_11.11.19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3C170C-73F0-7946-A661-580B30787D1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932CF7BF-806D-874B-8D9F-2385CBD2977F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="79">
   <si>
     <t>libraryDate</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Brent_large_3d-25_GTAC_25_SIC_Index2_09_CGTCGCT_TGTGAGGT_S26_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>08.29.19</t>
   </si>
   <si>
     <t>Brent_small_3d-26_GTAC_26_SIC_Index2_09_TCAACTG_TGTGAGGT_S27_R1_001.fastq.gz</t>
@@ -664,7 +661,7 @@
   <dimension ref="A1:Y63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1929,7 +1926,7 @@
     </row>
     <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>12</v>
@@ -1959,7 +1956,7 @@
         <v>5031505</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
@@ -1978,7 +1975,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>12</v>
@@ -2008,7 +2005,7 @@
         <v>7231560</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -2027,7 +2024,7 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>12</v>
@@ -2057,7 +2054,7 @@
         <v>10213502</v>
       </c>
       <c r="K29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
@@ -2065,7 +2062,7 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>12</v>
@@ -2095,7 +2092,7 @@
         <v>6822014</v>
       </c>
       <c r="K30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
@@ -2103,7 +2100,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>12</v>
@@ -2133,7 +2130,7 @@
         <v>4341048</v>
       </c>
       <c r="K31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
@@ -2141,7 +2138,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>12</v>
@@ -2171,7 +2168,7 @@
         <v>6680365</v>
       </c>
       <c r="K32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
@@ -2179,7 +2176,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>12</v>
@@ -2209,7 +2206,7 @@
         <v>6844663</v>
       </c>
       <c r="K33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
@@ -2217,7 +2214,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>12</v>
@@ -2247,7 +2244,7 @@
         <v>3994543</v>
       </c>
       <c r="K34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
@@ -2255,7 +2252,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>12</v>
@@ -2285,7 +2282,7 @@
         <v>2257508</v>
       </c>
       <c r="K35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
@@ -2293,7 +2290,7 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>12</v>
@@ -2323,7 +2320,7 @@
         <v>18162855</v>
       </c>
       <c r="K36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
@@ -2331,7 +2328,7 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>12</v>
@@ -2361,7 +2358,7 @@
         <v>9140479</v>
       </c>
       <c r="K37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
@@ -2369,7 +2366,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>12</v>
@@ -2399,7 +2396,7 @@
         <v>36598293</v>
       </c>
       <c r="K38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
@@ -2407,7 +2404,7 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>12</v>
@@ -2437,7 +2434,7 @@
         <v>5237450</v>
       </c>
       <c r="K39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
@@ -2445,7 +2442,7 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>12</v>
@@ -2475,7 +2472,7 @@
         <v>34123859</v>
       </c>
       <c r="K40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
@@ -2483,7 +2480,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>12</v>
@@ -2513,7 +2510,7 @@
         <v>3595819</v>
       </c>
       <c r="K41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
@@ -2521,7 +2518,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>12</v>
@@ -2551,7 +2548,7 @@
         <v>3874045</v>
       </c>
       <c r="K42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
@@ -2559,7 +2556,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>12</v>
@@ -2589,7 +2586,7 @@
         <v>7222032</v>
       </c>
       <c r="K43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
@@ -2597,7 +2594,7 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>12</v>
@@ -2627,7 +2624,7 @@
         <v>4500388</v>
       </c>
       <c r="K44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
@@ -2635,7 +2632,7 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>12</v>
@@ -2665,14 +2662,14 @@
         <v>6121691</v>
       </c>
       <c r="K45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O45" s="3"/>
       <c r="Q45" s="6"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>12</v>
@@ -2702,14 +2699,14 @@
         <v>2717379</v>
       </c>
       <c r="K46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O46" s="3"/>
       <c r="Q46" s="6"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>12</v>
@@ -2739,14 +2736,14 @@
         <v>3559294</v>
       </c>
       <c r="K47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O47" s="3"/>
       <c r="Q47" s="6"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>12</v>
@@ -2776,14 +2773,14 @@
         <v>11938927</v>
       </c>
       <c r="K48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O48" s="3"/>
       <c r="Q48" s="6"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>12</v>
@@ -2813,14 +2810,14 @@
         <v>40713836</v>
       </c>
       <c r="K49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O49" s="3"/>
       <c r="Q49" s="6"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>12</v>
@@ -2850,14 +2847,14 @@
         <v>46339288</v>
       </c>
       <c r="K50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O50" s="3"/>
       <c r="Q50" s="6"/>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>12</v>
@@ -2887,14 +2884,14 @@
         <v>2799214</v>
       </c>
       <c r="K51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O51" s="3"/>
       <c r="Q51" s="6"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>12</v>
@@ -2924,14 +2921,14 @@
         <v>4112294</v>
       </c>
       <c r="K52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O52" s="3"/>
       <c r="Q52" s="6"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>12</v>
@@ -2961,14 +2958,14 @@
         <v>5844319</v>
       </c>
       <c r="K53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O53" s="3"/>
       <c r="Q53" s="6"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>12</v>
@@ -2998,14 +2995,14 @@
         <v>6132196</v>
       </c>
       <c r="K54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O54" s="3"/>
       <c r="Q54" s="6"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>12</v>
@@ -3035,14 +3032,14 @@
         <v>4521601</v>
       </c>
       <c r="K55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O55" s="3"/>
       <c r="Q55" s="6"/>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>12</v>
@@ -3072,14 +3069,14 @@
         <v>4796508</v>
       </c>
       <c r="K56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O56" s="3"/>
       <c r="Q56" s="6"/>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>12</v>
@@ -3109,14 +3106,14 @@
         <v>884346</v>
       </c>
       <c r="K57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O57" s="3"/>
       <c r="Q57" s="6"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>12</v>
@@ -3146,14 +3143,14 @@
         <v>5746575</v>
       </c>
       <c r="K58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O58" s="3"/>
       <c r="Q58" s="6"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>12</v>
@@ -3183,14 +3180,14 @@
         <v>7229787</v>
       </c>
       <c r="K59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O59" s="3"/>
       <c r="Q59" s="6"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>12</v>
@@ -3220,14 +3217,14 @@
         <v>5333709</v>
       </c>
       <c r="K60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O60" s="3"/>
       <c r="Q60" s="6"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>12</v>
@@ -3257,14 +3254,14 @@
         <v>44030131</v>
       </c>
       <c r="K61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O61" s="3"/>
       <c r="Q61" s="6"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>12</v>
@@ -3294,14 +3291,14 @@
         <v>43674917</v>
       </c>
       <c r="K62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O62" s="3"/>
       <c r="Q62" s="6"/>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>12</v>
@@ -3331,7 +3328,7 @@
         <v>1991285</v>
       </c>
       <c r="K63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O63" s="3"/>
       <c r="Q63" s="6"/>

</xml_diff>